<commit_message>
Added delete construction button $ deleted "small" image folder
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="668">
   <si>
     <t>ΣΕΙΡΕΣ</t>
   </si>
@@ -2019,6 +2019,9 @@
   </si>
   <si>
     <t>ΔAA-L</t>
+  </si>
+  <si>
+    <t>test-kasa</t>
   </si>
 </sst>
 </file>
@@ -2417,7 +2420,7 @@
   <dimension ref="A1:J523"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2814,6 +2817,9 @@
       </c>
       <c r="D18" s="11" t="s">
         <v>657</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>667</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>628</v>

</xml_diff>